<commit_message>
Atualização automática de PALMEIRA_DAS_MISSOES.xlsx
</commit_message>
<xml_diff>
--- a/PALMEIRA_DAS_MISSOES.xlsx
+++ b/PALMEIRA_DAS_MISSOES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{739D4261-6DBA-4075-9A72-A7FB38056DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C436CAF9-5756-47B4-B2A7-D3522C2B098A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,20 +22,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="6" r:id="rId7"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1205,7 +1192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1265,36 +1252,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1333,14 +1296,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1393,7 +1351,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{798639D2-1330-47FB-9920-DC92E08E60DE}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{2C4D11B8-0969-42C5-BDED-D4AAA258B05C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1423,10 +1381,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE3C5F2F-9099-4C97-A3CA-FB4ABCCC0EBA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDDC0599-DC13-486F-A1BB-38496576F55B}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1464,7 +1422,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5357AE8B-ADDD-42AC-98CC-27B621B7FA19}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8D51EF2-FF05-40CC-8A57-66FC2164F0B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1527,7 +1485,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42EC6CF1-5173-4D67-A818-41D1573540EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54EE6BAB-4142-41C4-8796-0DFA3617C8F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1546,7 +1504,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA5F5FCB-9056-CAAC-688B-C853BE573110}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BBD0CA7-109B-58B0-6985-387528CB6D04}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1595,7 +1553,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA581251-0C0C-FD76-0097-C141C0EAD125}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D311DBEF-AC5E-B15E-E67F-A1D9799205CC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1614,7 +1572,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5BEAE3A-9A94-EB9F-063A-1DD253851788}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE4C1227-1375-ACA6-40BF-7C3A7E3E82CF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1645,7 +1603,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{757B0944-EC00-A6EB-9E41-553AF431CB25}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE6942E3-A754-7DFC-6B27-407348D3A3A5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1676,7 +1634,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A444A32-19E8-9EC5-D0FC-961DDD47BDA9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA53A463-DC71-FBA2-91A5-DB0E320B3E1C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1719,7 +1677,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{747C0585-4CB6-4525-A1B5-E1564C2BD862}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8387570-FEA9-44AA-A088-E5AEE4958D81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1757,7 +1715,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46F31966-308B-43F5-9C93-0A8E3114320B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7147C19-478F-4145-AEF5-829FD196DB4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1800,7 +1758,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA8BA14B-9C87-4D31-9208-6903769767CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2256A222-3368-4E9A-A415-6E16B9CE0228}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2113,7 +2071,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1220056-C258-40E0-8AD3-D565589589DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E73848-908A-4229-AEBC-0110E3746E2C}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2125,98 +2083,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="40"/>
-    <col min="6" max="6" width="2" style="40" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="40" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="40"/>
+    <col min="1" max="5" width="12.5703125" style="37"/>
+    <col min="6" max="6" width="2" style="37" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="39"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="39"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="39"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="39"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="39"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="39"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="39"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="39"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="39"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="39"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="39"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="39"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="39"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="39"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="39"/>
+      <c r="F15" s="36"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="39"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="39"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="39"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="39"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="39"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="39"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="39"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="39"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="39"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="39"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="39"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="39"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="39"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="39"/>
+      <c r="F29" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5768,19 +5726,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>289</v>
       </c>
     </row>
@@ -5803,68 +5761,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>296</v>
       </c>
     </row>
@@ -5882,16 +5840,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5925,7 +5883,7 @@
       <c r="J1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>308</v>
       </c>
     </row>
@@ -5939,10 +5897,10 @@
       <c r="C2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="21">
         <v>24.12</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="21">
         <v>2.41</v>
       </c>
       <c r="F2" s="2">
@@ -5960,7 +5918,7 @@
       <c r="J2" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="22">
         <v>1897</v>
       </c>
     </row>
@@ -5974,10 +5932,10 @@
       <c r="C3" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="21">
         <v>134.74</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="21">
         <v>13.47</v>
       </c>
       <c r="F3" s="2">
@@ -5995,7 +5953,7 @@
       <c r="J3" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="22">
         <v>1897</v>
       </c>
     </row>
@@ -6009,10 +5967,10 @@
       <c r="C4" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="21">
         <v>184.9</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="21">
         <v>18.489999999999998</v>
       </c>
       <c r="F4" s="2">
@@ -6030,7 +5988,7 @@
       <c r="J4" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="22">
         <v>1897</v>
       </c>
     </row>
@@ -6044,10 +6002,10 @@
       <c r="C5" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="21">
         <v>75.900000000000006</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="21">
         <v>7.59</v>
       </c>
       <c r="F5" s="2">
@@ -6065,7 +6023,7 @@
       <c r="J5" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="22">
         <v>1897</v>
       </c>
     </row>
@@ -6079,10 +6037,10 @@
       <c r="C6" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="21">
         <v>75.900000000000006</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="21">
         <v>7.59</v>
       </c>
       <c r="F6" s="2">
@@ -6100,7 +6058,7 @@
       <c r="J6" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="22">
         <v>1897</v>
       </c>
     </row>
@@ -6114,10 +6072,10 @@
       <c r="C7" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="21">
         <v>75.900000000000006</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="21">
         <v>7.59</v>
       </c>
       <c r="F7" s="2">
@@ -6135,7 +6093,7 @@
       <c r="J7" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="22">
         <v>1897</v>
       </c>
     </row>
@@ -6149,10 +6107,10 @@
       <c r="C8" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <v>1768.99</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="21">
         <v>176.9</v>
       </c>
       <c r="F8" s="2">
@@ -6170,7 +6128,7 @@
       <c r="J8" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="22">
         <v>1897</v>
       </c>
     </row>
@@ -6184,10 +6142,10 @@
       <c r="C9" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <v>1556</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="21">
         <v>727.43</v>
       </c>
       <c r="F9" s="2">
@@ -6205,7 +6163,7 @@
       <c r="J9" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="22">
         <v>1897</v>
       </c>
     </row>
@@ -6219,10 +6177,10 @@
       <c r="C10" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <v>718</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <v>71.8</v>
       </c>
       <c r="F10" s="2">
@@ -6240,7 +6198,7 @@
       <c r="J10" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="22">
         <v>707</v>
       </c>
     </row>
@@ -6265,54 +6223,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>327</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>328</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>329</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="25" t="s">
         <v>331</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="23" t="s">
         <v>333</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="23" t="s">
         <v>334</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="23" t="s">
         <v>336</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="23" t="s">
         <v>337</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="23" t="s">
         <v>338</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="23" t="s">
         <v>339</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="23" t="s">
         <v>340</v>
       </c>
     </row>
@@ -6323,43 +6282,43 @@
       <c r="B2" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="26">
         <v>45139</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="27">
         <v>4126</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="27" t="s">
         <v>342</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="28">
         <v>8603</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="28">
         <v>1403</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="29" t="s">
         <v>343</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="29" t="s">
         <v>343</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>343</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="29" t="s">
         <v>343</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="29" t="s">
         <v>343</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="30" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6390,25 +6349,24 @@
       <c r="B1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>347</v>
       </c>
-      <c r="E1" s="35">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="32">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="B2" s="35">
         <v>119</v>
       </c>
-      <c r="F1" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="38">
-        <v>119</v>
-      </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>7.8693294537759556E-3</v>
       </c>
     </row>

</xml_diff>